<commit_message>
Update On Import Lecturers
</commit_message>
<xml_diff>
--- a/dist/XLSFiles/ezanaLMS_Lecturers.xlsx
+++ b/dist/XLSFiles/ezanaLMS_Lecturers.xlsx
@@ -20,34 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="151">
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">created_at</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="168">
   <si>
     <t xml:space="preserve">093d69fd815225919ef1a4911c3b54d1f134cc07</t>
   </si>
@@ -97,6 +70,9 @@
     <t xml:space="preserve">Lecturer 003</t>
   </si>
   <si>
+    <t xml:space="preserve">lec003@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127002, localhost</t>
   </si>
   <si>
@@ -112,6 +88,9 @@
     <t xml:space="preserve">Lecturer 004</t>
   </si>
   <si>
+    <t xml:space="preserve">lec004@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127003, localhost</t>
   </si>
   <si>
@@ -127,6 +106,9 @@
     <t xml:space="preserve">Lecturer 005</t>
   </si>
   <si>
+    <t xml:space="preserve">lec005@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127004, localhost</t>
   </si>
   <si>
@@ -142,6 +124,9 @@
     <t xml:space="preserve">Lecturer 006</t>
   </si>
   <si>
+    <t xml:space="preserve">lec006@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127005, localhost</t>
   </si>
   <si>
@@ -157,6 +142,9 @@
     <t xml:space="preserve">Lecturer 007</t>
   </si>
   <si>
+    <t xml:space="preserve">lec007@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127006, localhost</t>
   </si>
   <si>
@@ -172,6 +160,9 @@
     <t xml:space="preserve">Lecturer 008</t>
   </si>
   <si>
+    <t xml:space="preserve">lec008@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127007, localhost</t>
   </si>
   <si>
@@ -187,6 +178,9 @@
     <t xml:space="preserve">Lecturer 009</t>
   </si>
   <si>
+    <t xml:space="preserve">lec009@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127008, localhost</t>
   </si>
   <si>
@@ -202,6 +196,9 @@
     <t xml:space="preserve">Lecturer 010</t>
   </si>
   <si>
+    <t xml:space="preserve">lec0010@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127009, localhost</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
     <t xml:space="preserve">Lecturer 011</t>
   </si>
   <si>
+    <t xml:space="preserve">lec011@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127010, localhost</t>
   </si>
   <si>
@@ -232,6 +232,9 @@
     <t xml:space="preserve">Lecturer 012</t>
   </si>
   <si>
+    <t xml:space="preserve">lec012@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127011, localhost</t>
   </si>
   <si>
@@ -247,6 +250,9 @@
     <t xml:space="preserve">Lecturer 013</t>
   </si>
   <si>
+    <t xml:space="preserve">lec013@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127012, localhost</t>
   </si>
   <si>
@@ -262,6 +268,9 @@
     <t xml:space="preserve">Lecturer 014</t>
   </si>
   <si>
+    <t xml:space="preserve">lec014@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127013, localhost</t>
   </si>
   <si>
@@ -277,6 +286,9 @@
     <t xml:space="preserve">Lecturer 015</t>
   </si>
   <si>
+    <t xml:space="preserve">lec015@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127014, localhost</t>
   </si>
   <si>
@@ -292,6 +304,9 @@
     <t xml:space="preserve">Lecturer 016</t>
   </si>
   <si>
+    <t xml:space="preserve">lec016@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127015, localhost</t>
   </si>
   <si>
@@ -307,6 +322,9 @@
     <t xml:space="preserve">Lecturer 017</t>
   </si>
   <si>
+    <t xml:space="preserve">lec017@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127016, localhost</t>
   </si>
   <si>
@@ -322,6 +340,9 @@
     <t xml:space="preserve">Lecturer 018</t>
   </si>
   <si>
+    <t xml:space="preserve">lec018@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127017, localhost</t>
   </si>
   <si>
@@ -337,6 +358,9 @@
     <t xml:space="preserve">Lecturer 019</t>
   </si>
   <si>
+    <t xml:space="preserve">lec019@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127018, localhost</t>
   </si>
   <si>
@@ -352,6 +376,9 @@
     <t xml:space="preserve">Lecturer 020</t>
   </si>
   <si>
+    <t xml:space="preserve">lec020@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127019, localhost</t>
   </si>
   <si>
@@ -364,6 +391,9 @@
     <t xml:space="preserve">Lecturer 021</t>
   </si>
   <si>
+    <t xml:space="preserve">lec021@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127020, localhost</t>
   </si>
   <si>
@@ -379,6 +409,9 @@
     <t xml:space="preserve">Lecturer 022</t>
   </si>
   <si>
+    <t xml:space="preserve">lec022@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127021, localhost</t>
   </si>
   <si>
@@ -394,6 +427,9 @@
     <t xml:space="preserve">Lecturer 023</t>
   </si>
   <si>
+    <t xml:space="preserve">lec023@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127022, localhost</t>
   </si>
   <si>
@@ -409,6 +445,9 @@
     <t xml:space="preserve">Lecturer 024</t>
   </si>
   <si>
+    <t xml:space="preserve">lec024@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127023, localhost</t>
   </si>
   <si>
@@ -424,6 +463,9 @@
     <t xml:space="preserve">Lecturer 025</t>
   </si>
   <si>
+    <t xml:space="preserve">lec025@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127024, localhost</t>
   </si>
   <si>
@@ -439,6 +481,9 @@
     <t xml:space="preserve">Lecturer 026</t>
   </si>
   <si>
+    <t xml:space="preserve">lec026@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127025, localhost</t>
   </si>
   <si>
@@ -454,6 +499,9 @@
     <t xml:space="preserve">Lecturer 027</t>
   </si>
   <si>
+    <t xml:space="preserve">lec027@ezana.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">127026, localhost</t>
   </si>
   <si>
@@ -467,6 +515,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lecturer 028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lec028@ezana.org</t>
   </si>
   <si>
     <t xml:space="preserve">127027, localhost</t>
@@ -568,10 +619,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -595,165 +646,165 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="0" t="n">
+        <v>3456787654</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>2548907654</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="n">
+        <v>3456787655</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>23456789056</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>3456787654</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>2548907654</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3456787656</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>23456789057</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="H3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>3456787655</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>23456789056</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3456787657</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>23456789058</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="H4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>3456787656</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>23456789057</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="D5" s="0" t="n">
+        <v>3456787658</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>23456789059</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>3456787657</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>23456789058</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="n">
+        <v>3456787659</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>23456789060</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>3456787658</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>23456789059</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>19</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>35</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>36</v>
@@ -770,660 +821,631 @@
         <v>39</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>3456787659</v>
+        <v>3456787660</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>23456789060</v>
+        <v>23456789061</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>3456787660</v>
+        <v>3456787661</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>23456789061</v>
+        <v>23456789062</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>3456787661</v>
+        <v>3456787662</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>23456789062</v>
+        <v>23456789063</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>3456787662</v>
+        <v>3456787663</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>23456789063</v>
+        <v>23456789064</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>3456787663</v>
+        <v>3456787664</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>23456789064</v>
+        <v>23456789065</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>3456787664</v>
+        <v>3456787665</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>23456789065</v>
+        <v>23456789066</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>3456787665</v>
+        <v>3456787666</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>23456789066</v>
+        <v>23456789067</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>3456787666</v>
+        <v>3456787667</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>23456789067</v>
+        <v>23456789068</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>3456787667</v>
+        <v>3456787668</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>23456789068</v>
+        <v>23456789069</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>3456787668</v>
+        <v>3456787669</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>23456789069</v>
+        <v>23456789070</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>3456787669</v>
+        <v>3456787670</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>23456789070</v>
+        <v>23456789071</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>3456787670</v>
+        <v>3456787671</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>23456789071</v>
+        <v>23456789072</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>3456787671</v>
+        <v>3456787672</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>23456789072</v>
+        <v>23456789073</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>19</v>
+        <v>112</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>3456787672</v>
+        <v>3456787673</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>23456789073</v>
+        <v>23456789074</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>106</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>3456787673</v>
+        <v>3456787674</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>23456789074</v>
+        <v>23456789075</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>15</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>3456787674</v>
+        <v>3456787675</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>23456789075</v>
+        <v>23456789076</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>3456787675</v>
+        <v>3456787676</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>23456789076</v>
+        <v>23456789077</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>3456787676</v>
+        <v>3456787677</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>23456789077</v>
+        <v>23456789078</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>3456787677</v>
+        <v>3456787678</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>23456789078</v>
+        <v>23456789079</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>3456787678</v>
+        <v>3456787679</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>23456789079</v>
+        <v>23456789080</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>3456787679</v>
+        <v>3456787680</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>23456789080</v>
+        <v>23456789081</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>19</v>
+        <v>159</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>3456787680</v>
+        <v>3456787681</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>23456789081</v>
+        <v>23456789082</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>19</v>
+        <v>165</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>3456787681</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>23456789082</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>